<commit_message>
se añaden generacion de asserts
</commit_message>
<xml_diff>
--- a/Mapping.xlsx
+++ b/Mapping.xlsx
@@ -1205,16 +1205,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1409,1493 +1413,1493 @@
   </sheetPr>
   <dimension ref="A1:B185"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A56" activeCellId="0" sqref="A56:B65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="58.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="2" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="2" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="2" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="2" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="2" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="2" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="2" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="2" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="2" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="1" t="s">
+      <c r="A81" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="2" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="1" t="s">
+      <c r="A82" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="2" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="1" t="s">
+      <c r="A83" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="B83" s="2" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="1" t="s">
+      <c r="A84" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="B84" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="2" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="B86" s="2" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="1" t="s">
+      <c r="A87" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="2" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="1" t="s">
+      <c r="A88" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="B88" s="2" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="1" t="s">
+      <c r="A89" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="B89" s="2" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="1" t="s">
+      <c r="A90" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B91" s="1" t="s">
+      <c r="B91" s="2" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="1" t="s">
+      <c r="A92" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="2" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B93" s="1" t="s">
+      <c r="B93" s="2" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="1" t="s">
+      <c r="A94" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="B94" s="1" t="s">
+      <c r="B94" s="2" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" s="2" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="1" t="s">
+      <c r="A96" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="1" t="s">
+      <c r="A97" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="2" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="1" t="s">
+      <c r="A98" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B98" s="1" t="s">
+      <c r="B98" s="2" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="1" t="s">
+      <c r="A99" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="B99" s="1" t="s">
+      <c r="B99" s="2" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="B100" s="1" t="s">
+      <c r="B100" s="2" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="1" t="s">
+      <c r="A101" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B101" s="2" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="2" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="1" t="s">
+      <c r="A103" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B103" s="1" t="s">
+      <c r="B103" s="2" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="1" t="s">
+      <c r="A104" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="2" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="1" t="s">
+      <c r="A105" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="B105" s="1" t="s">
+      <c r="B105" s="2" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="1" t="s">
+      <c r="A106" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="2" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="1" t="s">
+      <c r="A107" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="2" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="1" t="s">
+      <c r="A108" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="2" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="B109" s="1" t="s">
+      <c r="B109" s="2" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="1" t="s">
+      <c r="A110" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="2" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="1" t="s">
+      <c r="A111" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="B111" s="1" t="s">
+      <c r="B111" s="2" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="1" t="s">
+      <c r="A112" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B112" s="1" t="s">
+      <c r="B112" s="2" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B113" s="1" t="s">
+      <c r="B113" s="2" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="1" t="s">
+      <c r="A114" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="2" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="s">
+      <c r="A115" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="B115" s="1" t="s">
+      <c r="B115" s="2" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="B116" s="1" t="s">
+      <c r="B116" s="2" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="1" t="s">
+      <c r="A117" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="2" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B118" s="1" t="s">
+      <c r="B118" s="2" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="s">
+      <c r="A119" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B119" s="1" t="s">
+      <c r="B119" s="2" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="s">
+      <c r="A120" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B120" s="1" t="s">
+      <c r="B120" s="2" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="s">
+      <c r="A121" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B121" s="1" t="s">
+      <c r="B121" s="2" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="s">
+      <c r="A122" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B122" s="1" t="s">
+      <c r="B122" s="2" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="s">
+      <c r="A123" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="2" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="1" t="s">
+      <c r="A124" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="B124" s="1" t="s">
+      <c r="B124" s="2" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="1" t="s">
+      <c r="A125" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B125" s="1" t="s">
+      <c r="B125" s="2" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="1" t="s">
+      <c r="A126" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="B126" s="1" t="s">
+      <c r="B126" s="2" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="1" t="s">
+      <c r="A127" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B127" s="1" t="s">
+      <c r="B127" s="2" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="s">
+      <c r="A128" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B128" s="2" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="1" t="s">
+      <c r="A129" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="B129" s="1" t="s">
+      <c r="B129" s="2" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="s">
+      <c r="A130" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="B130" s="1" t="s">
+      <c r="B130" s="2" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="s">
+      <c r="A131" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B131" s="1" t="s">
+      <c r="B131" s="2" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="s">
+      <c r="A132" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B132" s="1" t="s">
+      <c r="B132" s="2" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="s">
+      <c r="A133" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B133" s="1" t="s">
+      <c r="B133" s="2" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="s">
+      <c r="A134" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="B134" s="1" t="s">
+      <c r="B134" s="2" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="1" t="s">
+      <c r="A135" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B135" s="1" t="s">
+      <c r="B135" s="2" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="s">
+      <c r="A136" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" s="2" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="1" t="s">
+      <c r="A137" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" s="2" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="1" t="s">
+      <c r="A138" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" s="2" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="1" t="s">
+      <c r="A139" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" s="2" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="1" t="s">
+      <c r="A140" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" s="2" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="1" t="s">
+      <c r="A141" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" s="2" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="s">
+      <c r="A142" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" s="2" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="s">
+      <c r="A143" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B143" s="1" t="s">
+      <c r="B143" s="2" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="B144" s="1" t="s">
+      <c r="B144" s="2" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="1" t="s">
+      <c r="A145" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B145" s="1" t="s">
+      <c r="B145" s="2" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="1" t="s">
+      <c r="A146" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B146" s="1" t="s">
+      <c r="B146" s="2" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="1" t="s">
+      <c r="A147" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B147" s="1" t="s">
+      <c r="B147" s="2" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="1" t="s">
+      <c r="A148" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="B148" s="1" t="s">
+      <c r="B148" s="2" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="2" t="s">
+      <c r="A149" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B149" s="1" t="s">
+      <c r="B149" s="2" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="s">
+      <c r="A150" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B150" s="1" t="s">
+      <c r="B150" s="2" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="s">
+      <c r="A151" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B151" s="1" t="s">
+      <c r="B151" s="2" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="1" t="s">
+      <c r="A152" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="B152" s="1" t="s">
+      <c r="B152" s="2" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="1" t="s">
+      <c r="A153" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B153" s="1" t="s">
+      <c r="B153" s="2" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="1" t="s">
+      <c r="A154" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B154" s="1" t="s">
+      <c r="B154" s="2" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="1" t="s">
+      <c r="A155" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B155" s="1" t="s">
+      <c r="B155" s="2" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="1" t="s">
+      <c r="A156" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="B156" s="2" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="s">
+      <c r="A157" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="B157" s="2" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="s">
+      <c r="A158" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="B158" s="1" t="s">
+      <c r="B158" s="2" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="1" t="s">
+      <c r="A159" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="B159" s="1" t="s">
+      <c r="B159" s="2" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="1" t="s">
+      <c r="A160" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B160" s="1" t="s">
+      <c r="B160" s="2" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="s">
+      <c r="A161" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B161" s="1" t="s">
+      <c r="B161" s="2" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="s">
+      <c r="A162" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B162" s="2" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="1" t="s">
+      <c r="A163" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B163" s="1" t="s">
+      <c r="B163" s="2" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="1" t="s">
+      <c r="A164" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B164" s="1" t="s">
+      <c r="B164" s="2" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="1" t="s">
+      <c r="A165" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B165" s="1" t="s">
+      <c r="B165" s="2" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="1" t="s">
+      <c r="A166" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B166" s="2" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="1" t="s">
+      <c r="A167" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B167" s="1" t="s">
+      <c r="B167" s="2" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="s">
+      <c r="A168" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B168" s="2" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="s">
+      <c r="A169" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B169" s="1" t="s">
+      <c r="B169" s="2" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="1" t="s">
+      <c r="A170" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B170" s="1" t="s">
+      <c r="B170" s="2" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="1" t="s">
+      <c r="A171" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B171" s="1" t="s">
+      <c r="B171" s="2" t="s">
         <v>340</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="1" t="s">
+      <c r="A172" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B172" s="1" t="s">
+      <c r="B172" s="2" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="1" t="s">
+      <c r="A173" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B173" s="1" t="s">
+      <c r="B173" s="2" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="1" t="s">
+      <c r="A174" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="B174" s="1" t="s">
+      <c r="B174" s="2" t="s">
         <v>346</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="1" t="s">
+      <c r="A175" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="B175" s="1" t="s">
+      <c r="B175" s="2" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="s">
+      <c r="A176" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B176" s="1" t="s">
+      <c r="B176" s="2" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="s">
+      <c r="A177" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="B177" s="1" t="s">
+      <c r="B177" s="2" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="s">
+      <c r="A178" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="B178" s="1" t="s">
+      <c r="B178" s="2" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="s">
+      <c r="A179" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="B179" s="1" t="s">
+      <c r="B179" s="2" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="1" t="s">
+      <c r="A180" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="B180" s="1" t="s">
+      <c r="B180" s="2" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="s">
+      <c r="A181" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B181" s="2" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="1" t="s">
+      <c r="A182" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="B182" s="1" t="s">
+      <c r="B182" s="2" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="s">
+      <c r="A183" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="B183" s="1" t="s">
+      <c r="B183" s="2" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="s">
+      <c r="A184" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="B184" s="1" t="s">
+      <c r="B184" s="2" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="1" t="s">
+      <c r="A185" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="B185" s="1" t="s">
+      <c r="B185" s="2" t="s">
         <v>364</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor: ahora cada registro de excel es una instancia del modelo
</commit_message>
<xml_diff>
--- a/Mapping.xlsx
+++ b/Mapping.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="366">
   <si>
     <t xml:space="preserve">referenceNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRING</t>
   </si>
   <si>
     <t xml:space="preserve">account.id</t>
@@ -1205,7 +1208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1215,6 +1218,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1411,10 +1418,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B185"/>
+  <dimension ref="A1:C185"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A169" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D188" activeCellId="0" sqref="D188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1430,1477 +1437,2032 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
+      <c r="A2" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>5</v>
+      <c r="A4" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>9</v>
+      <c r="A6" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
+      <c r="A8" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>39</v>
+      <c r="A21" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
-        <v>77</v>
+      <c r="A40" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="3" t="s">
-        <v>107</v>
+      <c r="A55" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="3" t="s">
-        <v>115</v>
+      <c r="A59" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="3" t="s">
-        <v>167</v>
+      <c r="A85" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>214</v>
+        <v>215</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>216</v>
+        <v>217</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>218</v>
+        <v>219</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>220</v>
+        <v>221</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="3" t="s">
-        <v>229</v>
+      <c r="A116" s="4" t="s">
+        <v>230</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="3" t="s">
-        <v>233</v>
+      <c r="A118" s="4" t="s">
+        <v>234</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>234</v>
+        <v>235</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="2" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>240</v>
+        <v>241</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="2" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>244</v>
+        <v>245</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>248</v>
+        <v>249</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="2" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>250</v>
+        <v>251</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>254</v>
+        <v>255</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="2" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>256</v>
+        <v>257</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>258</v>
+        <v>259</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>260</v>
+        <v>261</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>262</v>
+        <v>263</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="2" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="2" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>266</v>
+        <v>267</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="2" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>268</v>
+        <v>269</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>270</v>
+        <v>271</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>274</v>
+        <v>275</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>276</v>
+        <v>277</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>278</v>
+        <v>279</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="2" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="3" t="s">
-        <v>285</v>
+      <c r="A144" s="4" t="s">
+        <v>286</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>292</v>
+        <v>293</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="3" t="s">
-        <v>295</v>
+      <c r="A149" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>310</v>
+        <v>311</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>316</v>
+        <v>317</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="2" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>324</v>
+        <v>325</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="2" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="2" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>328</v>
+        <v>329</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="2" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>330</v>
+        <v>331</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="2" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>332</v>
+        <v>333</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="2" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>338</v>
+        <v>339</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="2" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>340</v>
+        <v>341</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>342</v>
+        <v>343</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>344</v>
+        <v>345</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>346</v>
+        <v>347</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>348</v>
+        <v>349</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>352</v>
+        <v>353</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>354</v>
+        <v>355</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>356</v>
+        <v>357</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>358</v>
+        <v>359</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>